<commit_message>
Data cleaned version 2
</commit_message>
<xml_diff>
--- a/Energypricescleaned.xlsx
+++ b/Energypricescleaned.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -804,6 +804,52 @@
         <v>156.4</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>129.7</v>
+      </c>
+      <c r="C11">
+        <v>131.6</v>
+      </c>
+      <c r="D11">
+        <v>120</v>
+      </c>
+      <c r="E11">
+        <v>127.1</v>
+      </c>
+      <c r="F11">
+        <v>134</v>
+      </c>
+      <c r="G11">
+        <v>173.3</v>
+      </c>
+      <c r="H11">
+        <v>181.5</v>
+      </c>
+      <c r="I11">
+        <v>248.9</v>
+      </c>
+      <c r="J11">
+        <v>178.4</v>
+      </c>
+      <c r="K11">
+        <v>140.7</v>
+      </c>
+      <c r="L11">
+        <v>157.1</v>
+      </c>
+      <c r="M11">
+        <v>150.7</v>
+      </c>
+      <c r="N11">
+        <v>172.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned data (Gas and electricity prices)
</commit_message>
<xml_diff>
--- a/Energypricescleaned.xlsx
+++ b/Energypricescleaned.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,11 +423,6 @@
           <t>2024-S2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>2025-S1</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,9 +473,6 @@
       <c r="M3">
         <v>192.8</v>
       </c>
-      <c r="N3">
-        <v>182.3</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -524,9 +516,6 @@
       <c r="M4">
         <v>279.7</v>
       </c>
-      <c r="N4">
-        <v>259.8</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -570,9 +559,6 @@
       <c r="M5">
         <v>188.2</v>
       </c>
-      <c r="N5">
-        <v>180.7</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -616,9 +602,6 @@
       <c r="M6">
         <v>222.3</v>
       </c>
-      <c r="N6">
-        <v>189.7</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -662,9 +645,6 @@
       <c r="M7">
         <v>81.19999999999999</v>
       </c>
-      <c r="N7">
-        <v>81.90000000000001</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -708,9 +688,6 @@
       <c r="M8">
         <v>254.4</v>
       </c>
-      <c r="N8">
-        <v>266</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -754,9 +731,6 @@
       <c r="M9">
         <v>139.9</v>
       </c>
-      <c r="N9">
-        <v>148</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -800,9 +774,6 @@
       <c r="M10">
         <v>162.9</v>
       </c>
-      <c r="N10">
-        <v>156.4</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -845,9 +816,6 @@
       </c>
       <c r="M11">
         <v>150.7</v>
-      </c>
-      <c r="N11">
-        <v>172.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last Version of data cleaning
</commit_message>
<xml_diff>
--- a/Energypricescleaned.xlsx
+++ b/Energypricescleaned.xlsx
@@ -434,216 +434,216 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="B3">
-        <v>108.4</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="C3">
-        <v>104.2</v>
+        <v>79.8</v>
       </c>
       <c r="D3">
-        <v>95.10000000000001</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="E3">
-        <v>90.80000000000001</v>
+        <v>81.8</v>
       </c>
       <c r="F3">
-        <v>104</v>
+        <v>85.3</v>
       </c>
       <c r="G3">
-        <v>148.5</v>
+        <v>90.89999999999999</v>
       </c>
       <c r="H3">
-        <v>237.1</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="I3">
-        <v>363.6</v>
+        <v>95.60000000000001</v>
       </c>
       <c r="J3">
-        <v>297.6</v>
+        <v>94.8</v>
       </c>
       <c r="K3">
-        <v>184.6</v>
+        <v>99.30000000000001</v>
       </c>
       <c r="L3">
-        <v>188.3</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="M3">
-        <v>192.8</v>
+        <v>101.4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="B4">
-        <v>147.3</v>
+        <v>108.4</v>
       </c>
       <c r="C4">
-        <v>132.1</v>
+        <v>104.2</v>
       </c>
       <c r="D4">
-        <v>143</v>
+        <v>95.10000000000001</v>
       </c>
       <c r="E4">
-        <v>145.1</v>
+        <v>90.80000000000001</v>
       </c>
       <c r="F4">
-        <v>156.2</v>
+        <v>104</v>
       </c>
       <c r="G4">
-        <v>159.6</v>
+        <v>148.5</v>
       </c>
       <c r="H4">
-        <v>189.9</v>
+        <v>237.1</v>
       </c>
       <c r="I4">
-        <v>233.3</v>
+        <v>363.6</v>
       </c>
       <c r="J4">
-        <v>297.3</v>
+        <v>297.6</v>
       </c>
       <c r="K4">
-        <v>288.2</v>
+        <v>184.6</v>
       </c>
       <c r="L4">
-        <v>280.6</v>
+        <v>188.3</v>
       </c>
       <c r="M4">
-        <v>279.7</v>
+        <v>192.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B5">
-        <v>132.6</v>
+        <v>147.3</v>
       </c>
       <c r="C5">
-        <v>128.7</v>
+        <v>132.1</v>
       </c>
       <c r="D5">
-        <v>117.8</v>
+        <v>143</v>
       </c>
       <c r="E5">
-        <v>126</v>
+        <v>145.1</v>
       </c>
       <c r="F5">
-        <v>135.8</v>
+        <v>156.2</v>
       </c>
       <c r="G5">
-        <v>187.8</v>
+        <v>159.6</v>
       </c>
       <c r="H5">
-        <v>257.9</v>
+        <v>189.9</v>
       </c>
       <c r="I5">
-        <v>296.6</v>
+        <v>233.3</v>
       </c>
       <c r="J5">
-        <v>216.5</v>
+        <v>297.3</v>
       </c>
       <c r="K5">
-        <v>206.8</v>
+        <v>288.2</v>
       </c>
       <c r="L5">
-        <v>184.1</v>
+        <v>280.6</v>
       </c>
       <c r="M5">
-        <v>188.2</v>
+        <v>279.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B6">
-        <v>114.8</v>
+        <v>132.6</v>
       </c>
       <c r="C6">
+        <v>128.7</v>
+      </c>
+      <c r="D6">
+        <v>117.8</v>
+      </c>
+      <c r="E6">
         <v>126</v>
       </c>
-      <c r="D6">
-        <v>124.2</v>
-      </c>
-      <c r="E6">
-        <v>129.2</v>
-      </c>
       <c r="F6">
-        <v>128.9</v>
+        <v>135.8</v>
       </c>
       <c r="G6">
-        <v>135.6</v>
+        <v>187.8</v>
       </c>
       <c r="H6">
-        <v>156.6</v>
+        <v>257.9</v>
       </c>
       <c r="I6">
-        <v>172.3</v>
+        <v>296.6</v>
       </c>
       <c r="J6">
-        <v>189.3</v>
+        <v>216.5</v>
       </c>
       <c r="K6">
-        <v>216.1</v>
+        <v>206.8</v>
       </c>
       <c r="L6">
-        <v>221.9</v>
+        <v>184.1</v>
       </c>
       <c r="M6">
-        <v>222.3</v>
+        <v>188.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B7">
-        <v>88.2</v>
+        <v>114.8</v>
       </c>
       <c r="C7">
-        <v>86.40000000000001</v>
+        <v>126</v>
       </c>
       <c r="D7">
-        <v>81.19999999999999</v>
+        <v>124.2</v>
       </c>
       <c r="E7">
-        <v>79.39999999999999</v>
+        <v>129.2</v>
       </c>
       <c r="F7">
-        <v>79.5</v>
+        <v>128.9</v>
       </c>
       <c r="G7">
-        <v>79</v>
+        <v>135.6</v>
       </c>
       <c r="H7">
-        <v>74.59999999999999</v>
+        <v>156.6</v>
       </c>
       <c r="I7">
-        <v>85.3</v>
+        <v>172.3</v>
       </c>
       <c r="J7">
-        <v>91.09999999999999</v>
+        <v>189.3</v>
       </c>
       <c r="K7">
-        <v>89.09999999999999</v>
+        <v>216.1</v>
       </c>
       <c r="L7">
-        <v>86.09999999999999</v>
+        <v>221.9</v>
       </c>
       <c r="M7">
-        <v>81.19999999999999</v>
+        <v>222.3</v>
       </c>
     </row>
     <row r="8">

</xml_diff>